<commit_message>
Fixed typo in Tiers table
</commit_message>
<xml_diff>
--- a/Tier System/in progress/v02-01/NBO-Microscopy Metadata Tier System_v02-01.xlsx
+++ b/Tier System/in progress/v02-01/NBO-Microscopy Metadata Tier System_v02-01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/strambc/Documents/GitHub/MicroscopyMetadata4DNGuidelines_GitHub repo/Tier System/in progress/v02-00/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/strambc/Documents/GitHub/NBOMicroscopyMetadataSpecs/Tier System/stable version/v02-00/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B316FEC-2702-4447-AE87-F64E18217E1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AFB1EE-3A7E-2A46-9E97-9939CD6FF587}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28320" windowHeight="16740" tabRatio="914" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28320" windowHeight="16740" tabRatio="914" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tier system_v02-00" sheetId="12" r:id="rId1"/>
@@ -108,9 +108,6 @@
     <t>Reporting qualitative effects, or effects that require simple quantification including the identification of non-refractive limited objects followed by basic  feature extraction and statistical analysis</t>
   </si>
   <si>
-    <t>Identification and localization of refraction-limited particles, super-resolution microscopy, tracking of intracellular dynamics</t>
-  </si>
-  <si>
     <t>Full documentation of microscopic setup, image acquisition and quality control</t>
   </si>
   <si>
@@ -194,6 +191,9 @@
   </si>
   <si>
     <t>Detailed environmental control device, microscope table, light source, light source coupling, transmittance light path,  magnification, sample positioning, focusing,  autofocus, filter, dichroic, additional optics and detector hardware specification (e.g., lightsource spectral properties; objective correction properties; focusing device ZReproducibility, ZSettlingTime, ZResolution, etc.) and settings (e.g., illumination attenuation; objective temperature and iris aperture; immersion liquid measured refractive index; sample positioning settings; detector integration; ligthpath configuration)</t>
+  </si>
+  <si>
+    <t>Identification and localization of diffraction-limited particles, super-resolution microscopy, tracking of intracellular dynamics</t>
   </si>
 </sst>
 </file>
@@ -885,6 +885,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -920,9 +923,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="35">
@@ -1334,7 +1334,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="47" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="64" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="63"/>
       <c r="C1" s="65"/>
@@ -1364,13 +1364,13 @@
         <v>2</v>
       </c>
       <c r="E2" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="62" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="62" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H2" s="62" t="s">
         <v>16</v>
@@ -1403,31 +1403,31 @@
         <v>20</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" s="41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J3" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="71" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="72"/>
+      <c r="L3" s="73"/>
       <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:13" s="10" customFormat="1" ht="406" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="68" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="29">
@@ -1437,34 +1437,34 @@
         <v>17</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="E4" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I4" s="45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J4" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="73" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="74"/>
+      <c r="K4" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="75"/>
       <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" s="11" customFormat="1" ht="343" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="68"/>
+      <c r="A5" s="69"/>
       <c r="B5" s="17">
         <v>3</v>
       </c>
@@ -1472,26 +1472,26 @@
         <v>18</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="69"/>
-      <c r="I5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="71"/>
       <c r="J5" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="70" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" s="75"/>
+      <c r="K5" s="71" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="76"/>
       <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:13" ht="29" customHeight="1" x14ac:dyDescent="0.35">
@@ -1521,8 +1521,8 @@
   </sheetPr>
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="89" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="57" zoomScaleNormal="89" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="29" x14ac:dyDescent="0.35"/>
@@ -1541,18 +1541,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
+      <c r="A1" s="79" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
     </row>
     <row r="2" spans="1:11" s="23" customFormat="1" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
@@ -1568,13 +1568,13 @@
         <v>2</v>
       </c>
       <c r="E2" s="58" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="79" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="67" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="58" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H2" s="58" t="s">
         <v>16</v>
@@ -1601,27 +1601,27 @@
         <v>20</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J3" s="35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" s="10" customFormat="1" ht="359" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="68" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="29">
@@ -1631,30 +1631,30 @@
         <v>17</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J4" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11" s="11" customFormat="1" ht="252" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="68"/>
+      <c r="A5" s="69"/>
       <c r="B5" s="17">
         <v>3</v>
       </c>
@@ -1662,21 +1662,21 @@
         <v>18</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="76" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="76"/>
-      <c r="I5" s="77"/>
+        <v>31</v>
+      </c>
+      <c r="G5" s="77" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="77"/>
+      <c r="I5" s="78"/>
       <c r="J5" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K5" s="7"/>
     </row>
@@ -1705,8 +1705,8 @@
   </sheetPr>
   <dimension ref="A2:I6"/>
   <sheetViews>
-    <sheetView zoomScale="56" zoomScaleNormal="72" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="72" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="29" x14ac:dyDescent="0.35"/>
@@ -1736,13 +1736,13 @@
         <v>2</v>
       </c>
       <c r="E2" s="58" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="58" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="58" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H2" s="58" t="s">
         <v>15</v>
@@ -1759,23 +1759,23 @@
         <v>19</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" s="49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H3" s="49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="10" customFormat="1" ht="370" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="68" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="29">
@@ -1785,23 +1785,23 @@
         <v>17</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H4" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="11" customFormat="1" ht="158" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="68"/>
+      <c r="A5" s="69"/>
       <c r="B5" s="17">
         <v>3</v>
       </c>
@@ -1809,19 +1809,19 @@
         <v>18</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="51" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H5" s="54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5"/>
     </row>

</xml_diff>